<commit_message>
Hinzufügung: Dokumentationsstatus; Bat Start Bug-Fixes; Regelunterteilung und Optimierung; UI angepasst
</commit_message>
<xml_diff>
--- a/backend/data/demo_cases.xlsx
+++ b/backend/data/demo_cases.xlsx
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -629,6 +629,16 @@
           <t>BSCL Austritt Suizidalität</t>
         </is>
       </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Fallstatus</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Fallführende Person</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -690,6 +700,16 @@
       <c r="Q2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="n">
@@ -750,6 +770,16 @@
       </c>
       <c r="Q3" s="4" t="n">
         <v>4</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -790,6 +820,16 @@
       <c r="O4" s="2" t="n"/>
       <c r="P4" s="2" t="n"/>
       <c r="Q4" s="2" t="n"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">
@@ -851,6 +891,16 @@
       <c r="Q5" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -898,6 +948,16 @@
       <c r="O6" s="2" t="n"/>
       <c r="P6" s="2" t="n"/>
       <c r="Q6" s="2" t="n"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="n">
@@ -945,6 +1005,16 @@
       <c r="O7" s="4" t="n"/>
       <c r="P7" s="4" t="n"/>
       <c r="Q7" s="4" t="n"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1006,6 +1076,16 @@
       <c r="Q8" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n">
@@ -1067,6 +1147,16 @@
       <c r="Q9" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1128,6 +1218,16 @@
       <c r="Q10" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n">
@@ -1177,6 +1277,16 @@
       <c r="O11" s="4" t="n"/>
       <c r="P11" s="4" t="n"/>
       <c r="Q11" s="4" t="n"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1238,6 +1348,16 @@
       <c r="Q12" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n">
@@ -1285,6 +1405,16 @@
       <c r="O13" s="4" t="n"/>
       <c r="P13" s="4" t="n"/>
       <c r="Q13" s="4" t="n"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1332,6 +1462,16 @@
       <c r="O14" s="2" t="n"/>
       <c r="P14" s="2" t="n"/>
       <c r="Q14" s="2" t="n"/>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="n">
@@ -1393,6 +1533,16 @@
       <c r="Q15" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1440,6 +1590,16 @@
       <c r="O16" s="2" t="n"/>
       <c r="P16" s="2" t="n"/>
       <c r="Q16" s="2" t="n"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="n">
@@ -1487,6 +1647,16 @@
       <c r="O17" s="4" t="n"/>
       <c r="P17" s="4" t="n"/>
       <c r="Q17" s="4" t="n"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1536,6 +1706,16 @@
       <c r="O18" s="2" t="n"/>
       <c r="P18" s="2" t="n"/>
       <c r="Q18" s="2" t="n"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="n">
@@ -1583,6 +1763,16 @@
       <c r="O19" s="4" t="n"/>
       <c r="P19" s="4" t="n"/>
       <c r="Q19" s="4" t="n"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1630,6 +1820,16 @@
       <c r="O20" s="2" t="n"/>
       <c r="P20" s="2" t="n"/>
       <c r="Q20" s="2" t="n"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n">
@@ -1691,6 +1891,16 @@
       <c r="Q21" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -1752,6 +1962,16 @@
       <c r="Q22" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n">
@@ -1801,6 +2021,16 @@
       <c r="O23" s="4" t="n"/>
       <c r="P23" s="4" t="n"/>
       <c r="Q23" s="4" t="n"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -1862,6 +2092,16 @@
       <c r="Q24" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="n">
@@ -1909,6 +2149,16 @@
       <c r="O25" s="4" t="n"/>
       <c r="P25" s="4" t="n"/>
       <c r="Q25" s="4" t="n"/>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -1956,6 +2206,16 @@
       <c r="O26" s="2" t="n"/>
       <c r="P26" s="2" t="n"/>
       <c r="Q26" s="2" t="n"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="n">
@@ -2017,6 +2277,16 @@
       <c r="Q27" s="4" t="n">
         <v>3</v>
       </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -2064,6 +2334,16 @@
       <c r="O28" s="2" t="n"/>
       <c r="P28" s="2" t="n"/>
       <c r="Q28" s="2" t="n"/>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="n">
@@ -2125,6 +2405,16 @@
       <c r="Q29" s="4" t="n">
         <v>4</v>
       </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -2185,6 +2475,16 @@
       </c>
       <c r="Q30" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -2227,6 +2527,16 @@
       <c r="O31" s="4" t="n"/>
       <c r="P31" s="4" t="n"/>
       <c r="Q31" s="4" t="n"/>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -2276,6 +2586,16 @@
       <c r="O32" s="2" t="n"/>
       <c r="P32" s="2" t="n"/>
       <c r="Q32" s="2" t="n"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="n">
@@ -2323,6 +2643,16 @@
       <c r="O33" s="4" t="n"/>
       <c r="P33" s="4" t="n"/>
       <c r="Q33" s="4" t="n"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -2370,6 +2700,16 @@
       <c r="O34" s="2" t="n"/>
       <c r="P34" s="2" t="n"/>
       <c r="Q34" s="2" t="n"/>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="n">
@@ -2417,6 +2757,16 @@
       <c r="O35" s="4" t="n"/>
       <c r="P35" s="4" t="n"/>
       <c r="Q35" s="4" t="n"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -2477,6 +2827,16 @@
       </c>
       <c r="Q36" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -2525,6 +2885,16 @@
         <v>3</v>
       </c>
       <c r="Q37" s="4" t="n"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -2572,6 +2942,16 @@
       <c r="O38" s="2" t="n"/>
       <c r="P38" s="2" t="n"/>
       <c r="Q38" s="2" t="n"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="n">
@@ -2613,6 +2993,16 @@
       <c r="O39" s="4" t="n"/>
       <c r="P39" s="4" t="n"/>
       <c r="Q39" s="4" t="n"/>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -2660,6 +3050,16 @@
       <c r="O40" s="2" t="n"/>
       <c r="P40" s="2" t="n"/>
       <c r="Q40" s="2" t="n"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="n">
@@ -2721,6 +3121,16 @@
       <c r="Q41" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -2768,6 +3178,16 @@
       <c r="O42" s="2" t="n"/>
       <c r="P42" s="2" t="n"/>
       <c r="Q42" s="2" t="n"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="4" t="n">
@@ -2809,6 +3229,16 @@
       <c r="O43" s="4" t="n"/>
       <c r="P43" s="4" t="n"/>
       <c r="Q43" s="4" t="n"/>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -2870,6 +3300,16 @@
       <c r="Q44" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="n">
@@ -2931,6 +3371,16 @@
       <c r="Q45" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -2992,6 +3442,16 @@
       <c r="Q46" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="4" t="n">
@@ -3039,6 +3499,16 @@
       <c r="O47" s="4" t="n"/>
       <c r="P47" s="4" t="n"/>
       <c r="Q47" s="4" t="n"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -3099,6 +3569,16 @@
       </c>
       <c r="Q48" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -3147,6 +3627,16 @@
         <v>3</v>
       </c>
       <c r="Q49" s="4" t="n"/>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -3196,6 +3686,16 @@
       <c r="O50" s="2" t="n"/>
       <c r="P50" s="2" t="n"/>
       <c r="Q50" s="2" t="n"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="4" t="n">
@@ -3257,6 +3757,16 @@
       <c r="Q51" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -3318,6 +3828,16 @@
       <c r="Q52" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="4" t="n">
@@ -3365,6 +3885,16 @@
       <c r="O53" s="4" t="n"/>
       <c r="P53" s="4" t="n"/>
       <c r="Q53" s="4" t="n"/>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -3414,6 +3944,16 @@
       <c r="O54" s="2" t="n"/>
       <c r="P54" s="2" t="n"/>
       <c r="Q54" s="2" t="n"/>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="4" t="n">
@@ -3461,6 +4001,16 @@
       <c r="O55" s="4" t="n"/>
       <c r="P55" s="4" t="n"/>
       <c r="Q55" s="4" t="n"/>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -3508,6 +4058,16 @@
       <c r="O56" s="2" t="n"/>
       <c r="P56" s="2" t="n"/>
       <c r="Q56" s="2" t="n"/>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="4" t="n">
@@ -3569,6 +4129,16 @@
       <c r="Q57" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -3630,6 +4200,16 @@
       <c r="Q58" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="4" t="n">
@@ -3677,6 +4257,16 @@
       <c r="O59" s="4" t="n"/>
       <c r="P59" s="4" t="n"/>
       <c r="Q59" s="4" t="n"/>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -3724,6 +4314,16 @@
       <c r="O60" s="2" t="n"/>
       <c r="P60" s="2" t="n"/>
       <c r="Q60" s="2" t="n"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="4" t="n">
@@ -3785,6 +4385,16 @@
       <c r="Q61" s="4" t="n">
         <v>2</v>
       </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -3832,6 +4442,16 @@
       <c r="O62" s="2" t="n"/>
       <c r="P62" s="2" t="n"/>
       <c r="Q62" s="2" t="n"/>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="4" t="n">
@@ -3893,6 +4513,16 @@
       <c r="Q63" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -3954,6 +4584,16 @@
       <c r="Q64" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="4" t="n">
@@ -4001,6 +4641,16 @@
       <c r="O65" s="4" t="n"/>
       <c r="P65" s="4" t="n"/>
       <c r="Q65" s="4" t="n"/>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -4062,6 +4712,16 @@
       <c r="Q66" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="4" t="n">
@@ -4123,6 +4783,16 @@
       <c r="Q67" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -4183,6 +4853,16 @@
       </c>
       <c r="Q68" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -4223,6 +4903,16 @@
       <c r="O69" s="4" t="n"/>
       <c r="P69" s="4" t="n"/>
       <c r="Q69" s="4" t="n"/>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -4284,6 +4974,16 @@
       <c r="Q70" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="4" t="n">
@@ -4345,6 +5045,16 @@
       <c r="Q71" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -4392,6 +5102,16 @@
       <c r="O72" s="2" t="n"/>
       <c r="P72" s="2" t="n"/>
       <c r="Q72" s="2" t="n"/>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="4" t="n">
@@ -4453,6 +5173,16 @@
       <c r="Q73" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -4500,6 +5230,16 @@
       <c r="O74" s="2" t="n"/>
       <c r="P74" s="2" t="n"/>
       <c r="Q74" s="2" t="n"/>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="4" t="n">
@@ -4560,6 +5300,16 @@
       </c>
       <c r="Q75" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -4602,6 +5352,16 @@
       <c r="O76" s="2" t="n"/>
       <c r="P76" s="2" t="n"/>
       <c r="Q76" s="2" t="n"/>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="4" t="n">
@@ -4663,6 +5423,16 @@
       <c r="Q77" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -4710,6 +5480,16 @@
       <c r="O78" s="2" t="n"/>
       <c r="P78" s="2" t="n"/>
       <c r="Q78" s="2" t="n"/>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="4" t="n">
@@ -4757,6 +5537,16 @@
       <c r="O79" s="4" t="n"/>
       <c r="P79" s="4" t="n"/>
       <c r="Q79" s="4" t="n"/>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -4804,6 +5594,16 @@
       <c r="O80" s="2" t="n"/>
       <c r="P80" s="2" t="n"/>
       <c r="Q80" s="2" t="n"/>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="4" t="n">
@@ -4853,6 +5653,16 @@
       <c r="O81" s="4" t="n"/>
       <c r="P81" s="4" t="n"/>
       <c r="Q81" s="4" t="n"/>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -4900,6 +5710,16 @@
       <c r="O82" s="2" t="n"/>
       <c r="P82" s="2" t="n"/>
       <c r="Q82" s="2" t="n"/>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="4" t="n">
@@ -4941,6 +5761,16 @@
       <c r="O83" s="4" t="n"/>
       <c r="P83" s="4" t="n"/>
       <c r="Q83" s="4" t="n"/>
+      <c r="R83" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -4988,6 +5818,16 @@
       <c r="O84" s="2" t="n"/>
       <c r="P84" s="2" t="n"/>
       <c r="Q84" s="2" t="n"/>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>Dr. Bauer</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="4" t="n">
@@ -5049,6 +5889,16 @@
       <c r="Q85" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="R85" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -5098,6 +5948,16 @@
       <c r="O86" s="2" t="n"/>
       <c r="P86" s="2" t="n"/>
       <c r="Q86" s="2" t="n"/>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="4" t="n">
@@ -5145,6 +6005,16 @@
       <c r="O87" s="4" t="n"/>
       <c r="P87" s="4" t="n"/>
       <c r="Q87" s="4" t="n"/>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -5192,6 +6062,16 @@
       <c r="O88" s="2" t="n"/>
       <c r="P88" s="2" t="n"/>
       <c r="Q88" s="2" t="n"/>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="4" t="n">
@@ -5239,6 +6119,16 @@
       <c r="O89" s="4" t="n"/>
       <c r="P89" s="4" t="n"/>
       <c r="Q89" s="4" t="n"/>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -5286,6 +6176,16 @@
       <c r="O90" s="2" t="n"/>
       <c r="P90" s="2" t="n"/>
       <c r="Q90" s="2" t="n"/>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>Dr. Fischer</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="4" t="n">
@@ -5333,6 +6233,16 @@
       <c r="O91" s="4" t="n"/>
       <c r="P91" s="4" t="n"/>
       <c r="Q91" s="4" t="n"/>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -5393,6 +6303,16 @@
       </c>
       <c r="Q92" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
       </c>
     </row>
     <row r="93">
@@ -5435,6 +6355,16 @@
       <c r="O93" s="4" t="n"/>
       <c r="P93" s="4" t="n"/>
       <c r="Q93" s="4" t="n"/>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
@@ -5476,6 +6406,16 @@
       <c r="O94" s="2" t="n"/>
       <c r="P94" s="2" t="n"/>
       <c r="Q94" s="2" t="n"/>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>Dokumentation offen</t>
+        </is>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="4" t="n">
@@ -5523,6 +6463,16 @@
       <c r="O95" s="4" t="n"/>
       <c r="P95" s="4" t="n"/>
       <c r="Q95" s="4" t="n"/>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
@@ -5584,6 +6534,16 @@
       <c r="Q96" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="4" t="n">
@@ -5631,6 +6591,16 @@
       <c r="O97" s="4" t="n"/>
       <c r="P97" s="4" t="n"/>
       <c r="Q97" s="4" t="n"/>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>Pfl. Weber</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
@@ -5678,6 +6648,16 @@
       <c r="O98" s="2" t="n"/>
       <c r="P98" s="2" t="n"/>
       <c r="Q98" s="2" t="n"/>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="4" t="n">
@@ -5739,6 +6719,16 @@
       <c r="Q99" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>Dokumentation abgeschlossen</t>
+        </is>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>Pfl. Schmidt</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -5786,6 +6776,16 @@
       <c r="O100" s="2" t="n"/>
       <c r="P100" s="2" t="n"/>
       <c r="Q100" s="2" t="n"/>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>Dr. Müller</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="4" t="n">
@@ -5833,6 +6833,16 @@
       <c r="O101" s="4" t="n"/>
       <c r="P101" s="4" t="n"/>
       <c r="Q101" s="4" t="n"/>
+      <c r="R101" t="inlineStr">
+        <is>
+          <t>Fall offen</t>
+        </is>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>Pfl. Meier</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1"/>

</xml_diff>